<commit_message>
Added RESET and 1PPS pins at PB4 and PB5
</commit_message>
<xml_diff>
--- a/Pin connections.xlsx
+++ b/Pin connections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Atollic\TrueSTUDIO\STM32_workspace_9.0\LoRa Mesh\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Atollic\TrueSTUDIO\STM32_workspace_9.0\LoRa Mesh CubeMX\Src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4D72336-F254-4424-8E8E-AA9B74CBEE7D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70B9C65-E75D-4834-9FAB-1AF8D931938E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{F7D98F9C-E68F-4E26-89E4-29FEB0C41D7C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{F7D98F9C-E68F-4E26-89E4-29FEB0C41D7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>STM32</t>
   </si>
@@ -109,6 +109,30 @@
   </si>
   <si>
     <t>TX</t>
+  </si>
+  <si>
+    <t>EXTI / PB1</t>
+  </si>
+  <si>
+    <t>EXTI / PB2</t>
+  </si>
+  <si>
+    <t>DIO2</t>
+  </si>
+  <si>
+    <t>DIO0</t>
+  </si>
+  <si>
+    <t>PB4</t>
+  </si>
+  <si>
+    <t>PB5</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>1PPS</t>
   </si>
 </sst>
 </file>
@@ -463,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265051B7-270C-46AE-9DED-CB4FCFD58D1A}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +545,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -604,21 +628,27 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -626,52 +656,90 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Layer 2 protocol
Most of the way through adding the layer two protocol but haven't tested anything yet
</commit_message>
<xml_diff>
--- a/Pin connections.xlsx
+++ b/Pin connections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Atollic\TrueSTUDIO\STM32_workspace_9.0\LoRa Mesh CubeMX\Src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70B9C65-E75D-4834-9FAB-1AF8D931938E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D4F343-B2F2-435B-BA5E-5C34B68379F6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{F7D98F9C-E68F-4E26-89E4-29FEB0C41D7C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
   <si>
     <t>STM32</t>
   </si>
@@ -75,18 +75,9 @@
     <t>GND</t>
   </si>
   <si>
-    <t>5V</t>
-  </si>
-  <si>
     <t>3.3V</t>
   </si>
   <si>
-    <t>3V</t>
-  </si>
-  <si>
-    <t>VIN</t>
-  </si>
-  <si>
     <t>UART 1</t>
   </si>
   <si>
@@ -133,6 +124,33 @@
   </si>
   <si>
     <t>1PPS</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>PB9</t>
+  </si>
+  <si>
+    <t>NRESET</t>
+  </si>
+  <si>
+    <t>CHECKED</t>
+  </si>
+  <si>
+    <t>DEBUG</t>
+  </si>
+  <si>
+    <t>NRST</t>
+  </si>
+  <si>
+    <t>SWCLK/PA14</t>
+  </si>
+  <si>
+    <t>SWDIO/PA13</t>
   </si>
 </sst>
 </file>
@@ -148,12 +166,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -168,11 +210,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265051B7-270C-46AE-9DED-CB4FCFD58D1A}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +561,7 @@
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,235 +575,368 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="C21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>